<commit_message>
Admin Request status update capability
</commit_message>
<xml_diff>
--- a/php/downloads/templates/sessions_template.xlsx
+++ b/php/downloads/templates/sessions_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UdithG\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp\www\jobshadowing\php\downloads\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -52,7 +52,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -113,11 +113,11 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -401,10 +401,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -437,9 +437,7 @@
       <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H2" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>